<commit_message>
Added login functionality to twitter
</commit_message>
<xml_diff>
--- a/files/data.xlsx
+++ b/files/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alan\Desktop\mqrs-top-img-gen\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4600D8BF-CC2B-4609-8DEE-07C58F06C8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33A2EAE-A5A5-4A77-8E71-1CFFA6CE34FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,9 +262,6 @@
     <t>2023/05/21 1:33:23 a.Â m. GMT-6</t>
   </si>
   <si>
-    <t>kevoiq</t>
-  </si>
-  <si>
     <t>2023/05/21 10:55:49 a.Â m. GMT-6</t>
   </si>
   <si>
@@ -379,9 +376,6 @@
     <t>2023/05/26 8:31:31 a.Â m. GMT-6</t>
   </si>
   <si>
-    <t>@MessiSan</t>
-  </si>
-  <si>
     <t>2023/05/26 2:58:14 p.Â m. GMT-6</t>
   </si>
   <si>
@@ -515,6 +509,12 @@
   </si>
   <si>
     <t>debufz</t>
+  </si>
+  <si>
+    <t>thatsgoodweb</t>
+  </si>
+  <si>
+    <t>70sscifi</t>
   </si>
 </sst>
 </file>
@@ -1411,8 +1411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,7 +1606,7 @@
         <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C2">
         <v>8.5</v>
@@ -1743,7 +1743,7 @@
         <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C3">
         <v>9</v>
@@ -2428,7 +2428,7 @@
         <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -3387,7 +3387,7 @@
         <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C15">
         <v>10</v>
@@ -4209,7 +4209,7 @@
         <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>163</v>
       </c>
       <c r="C21">
         <v>8.5</v>
@@ -4343,10 +4343,10 @@
     </row>
     <row r="22" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" t="s">
         <v>81</v>
-      </c>
-      <c r="B22" t="s">
-        <v>82</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -4480,10 +4480,10 @@
     </row>
     <row r="23" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" t="s">
         <v>83</v>
-      </c>
-      <c r="B23" t="s">
-        <v>84</v>
       </c>
       <c r="C23">
         <v>9</v>
@@ -4617,10 +4617,10 @@
     </row>
     <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C24">
         <v>9.3000000000000007</v>
@@ -4754,10 +4754,10 @@
     </row>
     <row r="25" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" t="s">
         <v>86</v>
-      </c>
-      <c r="B25" t="s">
-        <v>87</v>
       </c>
       <c r="C25">
         <v>9</v>
@@ -4891,10 +4891,10 @@
     </row>
     <row r="26" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
         <v>88</v>
-      </c>
-      <c r="B26" t="s">
-        <v>89</v>
       </c>
       <c r="C26">
         <v>10</v>
@@ -5028,10 +5028,10 @@
     </row>
     <row r="27" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" t="s">
         <v>90</v>
-      </c>
-      <c r="B27" t="s">
-        <v>91</v>
       </c>
       <c r="C27">
         <v>9.9</v>
@@ -5165,10 +5165,10 @@
     </row>
     <row r="28" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
         <v>92</v>
-      </c>
-      <c r="B28" t="s">
-        <v>93</v>
       </c>
       <c r="C28">
         <v>7.5</v>
@@ -5302,10 +5302,10 @@
     </row>
     <row r="29" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" t="s">
         <v>94</v>
-      </c>
-      <c r="B29" t="s">
-        <v>95</v>
       </c>
       <c r="C29">
         <v>9</v>
@@ -5439,10 +5439,10 @@
     </row>
     <row r="30" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" t="s">
         <v>96</v>
-      </c>
-      <c r="B30" t="s">
-        <v>97</v>
       </c>
       <c r="C30">
         <v>9.5</v>
@@ -5576,10 +5576,10 @@
     </row>
     <row r="31" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" t="s">
         <v>98</v>
-      </c>
-      <c r="B31" t="s">
-        <v>99</v>
       </c>
       <c r="C31">
         <v>9</v>
@@ -5713,10 +5713,10 @@
     </row>
     <row r="32" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
         <v>100</v>
-      </c>
-      <c r="B32" t="s">
-        <v>101</v>
       </c>
       <c r="C32">
         <v>10</v>
@@ -5850,10 +5850,10 @@
     </row>
     <row r="33" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" t="s">
         <v>102</v>
-      </c>
-      <c r="B33" t="s">
-        <v>103</v>
       </c>
       <c r="C33">
         <v>10</v>
@@ -5987,10 +5987,10 @@
     </row>
     <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" t="s">
         <v>104</v>
-      </c>
-      <c r="B34" t="s">
-        <v>105</v>
       </c>
       <c r="C34">
         <v>10</v>
@@ -6124,10 +6124,10 @@
     </row>
     <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" t="s">
         <v>106</v>
-      </c>
-      <c r="B35" t="s">
-        <v>107</v>
       </c>
       <c r="C35">
         <v>9</v>
@@ -6261,10 +6261,10 @@
     </row>
     <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" t="s">
         <v>108</v>
-      </c>
-      <c r="B36" t="s">
-        <v>109</v>
       </c>
       <c r="C36">
         <v>10</v>
@@ -6398,10 +6398,10 @@
     </row>
     <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" t="s">
         <v>110</v>
-      </c>
-      <c r="B37" t="s">
-        <v>111</v>
       </c>
       <c r="C37">
         <v>10</v>
@@ -6535,10 +6535,10 @@
     </row>
     <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" t="s">
         <v>112</v>
-      </c>
-      <c r="B38" t="s">
-        <v>113</v>
       </c>
       <c r="C38">
         <v>8.5</v>
@@ -6672,10 +6672,10 @@
     </row>
     <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" t="s">
         <v>114</v>
-      </c>
-      <c r="B39" t="s">
-        <v>115</v>
       </c>
       <c r="C39">
         <v>8.5</v>
@@ -6809,10 +6809,10 @@
     </row>
     <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" t="s">
         <v>116</v>
-      </c>
-      <c r="B40" t="s">
-        <v>117</v>
       </c>
       <c r="C40">
         <v>10</v>
@@ -6946,10 +6946,10 @@
     </row>
     <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
       <c r="C41">
         <v>9.5</v>
@@ -7083,10 +7083,10 @@
     </row>
     <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B42" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C42">
         <v>10</v>
@@ -7220,10 +7220,10 @@
     </row>
     <row r="43" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C43">
         <v>9</v>
@@ -7357,10 +7357,10 @@
     </row>
     <row r="44" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B44" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C44">
         <v>8</v>
@@ -7494,10 +7494,10 @@
     </row>
     <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B45" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C45">
         <v>10</v>
@@ -7631,10 +7631,10 @@
     </row>
     <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B46" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C46">
         <v>10</v>
@@ -7768,10 +7768,10 @@
     </row>
     <row r="47" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B47" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C47">
         <v>10</v>
@@ -7905,10 +7905,10 @@
     </row>
     <row r="48" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B48" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C48">
         <v>8.5</v>
@@ -8042,10 +8042,10 @@
     </row>
     <row r="49" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B49" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C49">
         <v>6.9</v>
@@ -8179,10 +8179,10 @@
     </row>
     <row r="50" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B50" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C50">
         <v>10</v>
@@ -8316,10 +8316,10 @@
     </row>
     <row r="51" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B51" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C51">
         <v>2.9</v>
@@ -8453,10 +8453,10 @@
     </row>
     <row r="52" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B52" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C52">
         <v>10</v>
@@ -8590,10 +8590,10 @@
     </row>
     <row r="53" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B53" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C53">
         <v>8.5</v>
@@ -8727,10 +8727,10 @@
     </row>
     <row r="54" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B54" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C54">
         <v>10</v>
@@ -8864,10 +8864,10 @@
     </row>
     <row r="55" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B55" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C55">
         <v>10</v>
@@ -9001,10 +9001,10 @@
     </row>
     <row r="56" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B56" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C56">
         <v>8</v>
@@ -9138,10 +9138,10 @@
     </row>
     <row r="57" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B57" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C57">
         <v>7</v>
@@ -9275,10 +9275,10 @@
     </row>
     <row r="58" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B58" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C58">
         <v>6.5</v>
@@ -9412,10 +9412,10 @@
     </row>
     <row r="59" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C59">
         <v>10</v>
@@ -9549,10 +9549,10 @@
     </row>
     <row r="60" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B60" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C60">
         <v>8</v>
@@ -9686,10 +9686,10 @@
     </row>
     <row r="61" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C61">
         <v>9.5</v>
@@ -9823,10 +9823,10 @@
     </row>
     <row r="62" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B62" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C62">
         <v>10</v>

</xml_diff>